<commit_message>
po przekształceniach i zaookrągleniach
</commit_message>
<xml_diff>
--- a/dane/Dane2.xlsx
+++ b/dane/Dane2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\Ekonometria_projekt\dane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F768CF-212B-461B-887E-11B51C654B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C0A7D1-C001-4CD9-946E-BB414709813F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1587B9EB-72E7-4C7E-BA4A-0E63A8296CF7}"/>
   </bookViews>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>L.p</t>
   </si>
   <si>
     <t>Lata</t>
-  </si>
-  <si>
-    <t>y - R&amp;D w milionach euro</t>
   </si>
   <si>
     <t>y - B+R na 1 mieszkanca</t>
@@ -60,12 +57,6 @@
     <t>x4 - Liczba_studentów na 1000 osób</t>
   </si>
   <si>
-    <t>x6 - Liczba_zarejstrowanych_startapów</t>
-  </si>
-  <si>
-    <t>x7 - Liczba_zgłoszonych_patentów</t>
-  </si>
-  <si>
     <t>x8 - Liczba osoób zatrudnionych w R&amp;D na 1000 osób pracujących</t>
   </si>
   <si>
@@ -73,6 +64,12 @@
   </si>
   <si>
     <t>x9 - Stopa_bezrobocia</t>
+  </si>
+  <si>
+    <t>x7 - Liczba_zgłoszonych_patentów_w_1000</t>
+  </si>
+  <si>
+    <t>x6 - Liczba_zarejstrowanych_startapów_w_1000</t>
   </si>
 </sst>
 </file>
@@ -148,21 +145,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,16 +474,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAF2763-4591-4F83-ACF8-5B34C9DC1611}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
@@ -497,704 +494,653 @@
     <col min="12" max="13" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>2023</v>
       </c>
-      <c r="C2" s="1">
-        <v>129972</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="6">
         <v>1560.66</v>
       </c>
-      <c r="E2" s="4">
+      <c r="D2" s="6">
         <v>49.52</v>
       </c>
-      <c r="F2" s="4">
+      <c r="E2" s="6">
         <v>0.48899999999999999</v>
       </c>
-      <c r="G2" s="4">
+      <c r="F2" s="6">
         <v>5.95</v>
       </c>
-      <c r="H2" s="5">
+      <c r="G2" s="5">
         <v>34.44177474</v>
       </c>
-      <c r="I2" s="6">
+      <c r="H2" s="7">
         <v>902.92313880883762</v>
       </c>
-      <c r="J2" s="5">
+      <c r="I2" s="5">
         <v>593.24400000000003</v>
       </c>
-      <c r="K2" s="8">
+      <c r="J2" s="3">
         <v>38.469000000000001</v>
       </c>
-      <c r="L2" s="5">
+      <c r="K2" s="5">
         <v>18.670442749999999</v>
       </c>
-      <c r="M2" s="4">
+      <c r="L2" s="6">
         <v>3.0680000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>2022</v>
       </c>
-      <c r="C3" s="2">
-        <v>121421.258</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" s="6">
         <v>1448.98</v>
       </c>
-      <c r="E3" s="4">
+      <c r="D3" s="6">
         <v>47.18</v>
       </c>
-      <c r="F3" s="4">
+      <c r="E3" s="6">
         <v>1.9800000000000002E-2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="F3" s="6">
         <v>6.87</v>
       </c>
-      <c r="H3" s="5">
+      <c r="G3" s="5">
         <v>34.848845109999999</v>
       </c>
-      <c r="I3" s="6">
+      <c r="H3" s="7">
         <v>845.52621402531338</v>
       </c>
-      <c r="J3" s="5">
+      <c r="I3" s="5">
         <v>554.81600000000003</v>
       </c>
-      <c r="K3" s="8">
+      <c r="J3" s="3">
         <v>37.204000000000001</v>
       </c>
-      <c r="L3" s="5">
+      <c r="K3" s="5">
         <v>17.86917047</v>
       </c>
-      <c r="M3" s="4">
+      <c r="L3" s="6">
         <v>3.12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>2021</v>
       </c>
-      <c r="C4" s="2">
-        <v>113183.57799999999</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="6">
         <v>1360.44</v>
       </c>
-      <c r="E4" s="4">
+      <c r="D4" s="6">
         <v>44.19</v>
       </c>
-      <c r="F4" s="4">
+      <c r="E4" s="6">
         <v>-5.8400000000000001E-2</v>
       </c>
-      <c r="G4" s="4">
+      <c r="F4" s="6">
         <v>3.07</v>
       </c>
-      <c r="H4" s="5">
+      <c r="G4" s="5">
         <v>35.3612222</v>
       </c>
-      <c r="I4" s="6">
+      <c r="H4" s="7">
         <v>807.74314866140685</v>
       </c>
-      <c r="J4" s="5">
+      <c r="I4" s="5">
         <v>583.13400000000001</v>
       </c>
-      <c r="K4" s="8">
+      <c r="J4" s="3">
         <v>39.829000000000001</v>
       </c>
-      <c r="L4" s="5">
+      <c r="K4" s="5">
         <v>17.418736169999999</v>
       </c>
-      <c r="M4" s="4">
+      <c r="L4" s="6">
         <v>3.5939999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>2020</v>
       </c>
-      <c r="C5" s="2">
-        <v>106582.97100000001</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="6">
         <v>1281.6500000000001</v>
       </c>
-      <c r="E5" s="4">
+      <c r="D5" s="6">
         <v>41.48</v>
       </c>
-      <c r="F5" s="4">
+      <c r="E5" s="6">
         <v>-5.8400000000000001E-2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="F5" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H5" s="5">
+      <c r="G5" s="5">
         <v>35.403008219999997</v>
       </c>
-      <c r="I5" s="6">
+      <c r="H5" s="7">
         <v>774.84247369174375</v>
       </c>
-      <c r="J5" s="5">
+      <c r="I5" s="5">
         <v>543.80600000000004</v>
       </c>
-      <c r="K5" s="8">
+      <c r="J5" s="3">
         <v>42.268999999999998</v>
       </c>
-      <c r="L5" s="5">
+      <c r="K5" s="5">
         <v>16.919189540000001</v>
       </c>
-      <c r="M5" s="4">
+      <c r="L5" s="6">
         <v>3.8809999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>2019</v>
       </c>
-      <c r="C6" s="2">
-        <v>110025.41</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="6">
         <v>1324.12</v>
       </c>
-      <c r="E6" s="4">
+      <c r="D6" s="6">
         <v>42.54</v>
       </c>
-      <c r="F6" s="4">
+      <c r="E6" s="6">
         <v>-5.0799999999999998E-2</v>
       </c>
-      <c r="G6" s="4">
+      <c r="F6" s="6">
         <v>1.45</v>
       </c>
-      <c r="H6" s="5">
+      <c r="G6" s="5">
         <v>34.792946720000003</v>
       </c>
-      <c r="I6" s="6">
+      <c r="H6" s="7">
         <v>734.26684440494489</v>
       </c>
-      <c r="J6" s="5">
+      <c r="I6" s="5">
         <v>550.56500000000005</v>
       </c>
-      <c r="K6" s="8">
+      <c r="J6" s="3">
         <v>46.631</v>
       </c>
-      <c r="L6" s="5">
+      <c r="K6" s="5">
         <v>16.724725110000001</v>
       </c>
-      <c r="M6" s="4">
+      <c r="L6" s="6">
         <v>3.1629999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>2018</v>
       </c>
-      <c r="C7" s="2">
-        <v>104669.045</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="6">
         <v>1262.51</v>
       </c>
-      <c r="E7" s="4">
+      <c r="D7" s="6">
         <v>41.39</v>
       </c>
-      <c r="F7" s="4">
+      <c r="E7" s="6">
         <v>-4.7E-2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="F7" s="6">
         <v>1.73</v>
       </c>
-      <c r="H7" s="5">
+      <c r="G7" s="5">
         <v>34.59616363</v>
       </c>
-      <c r="I7" s="6">
+      <c r="H7" s="7">
         <v>690.94322034137497</v>
       </c>
-      <c r="J7" s="5">
+      <c r="I7" s="5">
         <v>542.46100000000001</v>
       </c>
-      <c r="K7" s="8">
+      <c r="J7" s="3">
         <v>46.631</v>
       </c>
-      <c r="L7" s="5">
+      <c r="K7" s="5">
         <v>16.227081179999999</v>
       </c>
-      <c r="M7" s="4">
+      <c r="L7" s="6">
         <v>3.3839999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>2017</v>
       </c>
-      <c r="C8" s="2">
-        <v>99553.615999999995</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="6">
         <v>1204.42</v>
       </c>
-      <c r="E8" s="4">
+      <c r="D8" s="6">
         <v>40.299999999999997</v>
       </c>
-      <c r="F8" s="4">
+      <c r="E8" s="6">
         <v>-4.7E-2</v>
       </c>
-      <c r="G8" s="4">
+      <c r="F8" s="6">
         <v>1.51</v>
       </c>
-      <c r="H8" s="5">
+      <c r="G8" s="5">
         <v>34.419080430000001</v>
       </c>
-      <c r="I8" s="6">
+      <c r="H8" s="7">
         <v>654.88359957696025</v>
       </c>
-      <c r="J8" s="5">
+      <c r="I8" s="5">
         <v>549.678</v>
       </c>
-      <c r="K8" s="8">
+      <c r="J8" s="3">
         <v>47.786000000000001</v>
       </c>
-      <c r="L8" s="5">
+      <c r="K8" s="5">
         <v>15.817515179999999</v>
       </c>
-      <c r="M8" s="4">
+      <c r="L8" s="6">
         <v>3.7810000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>2016</v>
       </c>
-      <c r="C9" s="2">
-        <v>92173.555999999997</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9" s="6">
         <v>1119.31</v>
       </c>
-      <c r="E9" s="4">
+      <c r="D9" s="6">
         <v>38.81</v>
       </c>
-      <c r="F9" s="4">
+      <c r="E9" s="6">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="G9" s="4">
+      <c r="F9" s="6">
         <v>0.49</v>
       </c>
-      <c r="H9" s="5">
+      <c r="G9" s="5">
         <v>34.086889730000003</v>
       </c>
-      <c r="I9" s="6">
+      <c r="H9" s="7">
         <v>632.83999162147961</v>
       </c>
-      <c r="J9" s="5">
+      <c r="I9" s="5">
         <v>554.43600000000004</v>
       </c>
-      <c r="K9" s="8">
+      <c r="J9" s="3">
         <v>48.494</v>
       </c>
-      <c r="L9" s="5">
+      <c r="K9" s="5">
         <v>15.25797661</v>
       </c>
-      <c r="M9" s="4">
+      <c r="L9" s="6">
         <v>4.1040000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>2015</v>
       </c>
-      <c r="C10" s="2">
-        <v>88781.819000000003</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10" s="6">
         <v>1086.8599999999999</v>
       </c>
-      <c r="E10" s="4">
+      <c r="D10" s="6">
         <v>37.770000000000003</v>
       </c>
-      <c r="F10" s="4">
+      <c r="E10" s="6">
         <v>-2.47E-2</v>
       </c>
-      <c r="G10" s="4">
+      <c r="F10" s="6">
         <v>0.51</v>
       </c>
-      <c r="H10" s="5">
+      <c r="G10" s="5">
         <v>33.760722430000001</v>
       </c>
-      <c r="I10" s="6">
+      <c r="H10" s="7">
         <v>612.43835908433027</v>
       </c>
-      <c r="J10" s="5">
+      <c r="I10" s="5">
         <v>571.80899999999997</v>
       </c>
-      <c r="K10" s="8">
+      <c r="J10" s="3">
         <v>47.389000000000003</v>
       </c>
-      <c r="L10" s="5">
+      <c r="K10" s="5">
         <v>15.002692919999999</v>
       </c>
-      <c r="M10" s="4">
+      <c r="L10" s="6">
         <v>4.6120000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>2014</v>
       </c>
-      <c r="C11" s="2">
-        <v>84246.766000000003</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" s="6">
         <v>1040.31</v>
       </c>
-      <c r="E11" s="4">
+      <c r="D11" s="6">
         <v>36.86</v>
       </c>
-      <c r="F11" s="4">
+      <c r="E11" s="6">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="G11" s="4">
+      <c r="F11" s="6">
         <v>0.91</v>
       </c>
-      <c r="H11" s="5">
+      <c r="G11" s="5">
         <v>33.327076839999997</v>
       </c>
-      <c r="I11" s="6">
+      <c r="H11" s="7">
         <v>595.28159787608433</v>
       </c>
-      <c r="J11" s="5">
+      <c r="I11" s="5">
         <v>585.65599999999995</v>
       </c>
-      <c r="K11" s="8">
+      <c r="J11" s="3">
         <v>48.158000000000001</v>
       </c>
-      <c r="L11" s="5">
+      <c r="K11" s="5">
         <v>14.25746228</v>
       </c>
-      <c r="M11" s="4">
+      <c r="L11" s="6">
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>2013</v>
       </c>
-      <c r="C12" s="2">
-        <v>79729.508000000002</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="6">
         <v>988.64</v>
       </c>
-      <c r="E12" s="4">
+      <c r="D12" s="6">
         <v>35.549999999999997</v>
       </c>
-      <c r="F12" s="4">
+      <c r="E12" s="6">
         <v>0</v>
       </c>
-      <c r="G12" s="4">
+      <c r="F12" s="6">
         <v>1.5</v>
       </c>
-      <c r="H12" s="5">
+      <c r="G12" s="5">
         <v>32.449145860000002</v>
       </c>
-      <c r="I12" s="6">
+      <c r="H12" s="7">
         <v>574.29544982643506</v>
       </c>
-      <c r="J12" s="5">
+      <c r="I12" s="5">
         <v>615.596</v>
       </c>
-      <c r="K12" s="8">
+      <c r="J12" s="3">
         <v>47.591000000000001</v>
       </c>
-      <c r="L12" s="5">
+      <c r="K12" s="5">
         <v>13.954933349999999</v>
       </c>
-      <c r="M12" s="4">
+      <c r="L12" s="6">
         <v>5.3159999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>2012</v>
       </c>
-      <c r="C13" s="2">
-        <v>79110.377999999997</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="6">
         <v>983.64</v>
       </c>
-      <c r="E13" s="4">
+      <c r="D13" s="6">
         <v>34.82</v>
       </c>
-      <c r="F13" s="4">
+      <c r="E13" s="6">
         <v>1.5100000000000001E-2</v>
       </c>
-      <c r="G13" s="4">
+      <c r="F13" s="6">
         <v>2.0099999999999998</v>
       </c>
-      <c r="H13" s="5">
+      <c r="G13" s="5">
         <v>31.077195190000001</v>
       </c>
-      <c r="I13" s="6">
+      <c r="H13" s="7">
         <v>559.66747147865681</v>
       </c>
-      <c r="J13" s="5">
+      <c r="I13" s="5">
         <v>618.78</v>
       </c>
-      <c r="K13" s="8">
+      <c r="J13" s="3">
         <v>46.904000000000003</v>
       </c>
-      <c r="L13" s="5">
+      <c r="K13" s="5">
         <v>14.15704433</v>
       </c>
-      <c r="M13" s="4">
+      <c r="L13" s="6">
         <v>5.3719999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="5">
         <v>2011</v>
       </c>
-      <c r="C14" s="2">
-        <v>75569.073000000004</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="6">
         <v>941.38</v>
       </c>
-      <c r="E14" s="4">
+      <c r="D14" s="6">
         <v>34.229999999999997</v>
       </c>
-      <c r="F14" s="4">
+      <c r="E14" s="6">
         <v>6.1699999999999998E-2</v>
       </c>
-      <c r="G14" s="4">
+      <c r="F14" s="6">
         <v>2.08</v>
       </c>
-      <c r="H14" s="5">
+      <c r="G14" s="5">
         <v>29.660224280000001</v>
       </c>
-      <c r="I14" s="6">
+      <c r="H14" s="7">
         <v>543.94916533336425</v>
       </c>
-      <c r="J14" s="5">
+      <c r="I14" s="5">
         <v>679.06799999999998</v>
       </c>
-      <c r="K14" s="8">
+      <c r="J14" s="3">
         <v>47.241</v>
       </c>
-      <c r="L14" s="5">
+      <c r="K14" s="5">
         <v>13.850237659999999</v>
       </c>
-      <c r="M14" s="4">
+      <c r="L14" s="6">
         <v>5.9669999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="5">
         <v>2010</v>
       </c>
-      <c r="C15" s="2">
-        <v>70014.207999999999</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15" s="6">
         <v>856.16</v>
       </c>
-      <c r="E15" s="4">
+      <c r="D15" s="6">
         <v>32.590000000000003</v>
       </c>
-      <c r="F15" s="4">
+      <c r="E15" s="6">
         <v>3.04E-2</v>
       </c>
-      <c r="G15" s="4">
+      <c r="F15" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H15" s="5">
+      <c r="G15" s="5">
         <v>27.113930539999998</v>
       </c>
-      <c r="I15" s="6">
+      <c r="H15" s="7">
         <v>503.19266081522011</v>
       </c>
-      <c r="J15" s="5">
+      <c r="I15" s="5">
         <v>719.65300000000002</v>
       </c>
-      <c r="K15" s="8">
+      <c r="J15" s="3">
         <v>47.487000000000002</v>
       </c>
-      <c r="L15" s="5">
+      <c r="K15" s="5">
         <v>13.10836183</v>
       </c>
-      <c r="M15" s="4">
+      <c r="L15" s="6">
         <v>7.0430000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="5">
         <v>2009</v>
       </c>
-      <c r="C16" s="2">
-        <v>67078.120999999999</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16" s="6">
         <v>819</v>
       </c>
-      <c r="E16" s="4">
+      <c r="D16" s="6">
         <v>31</v>
       </c>
-      <c r="F16" s="4">
+      <c r="E16" s="6">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="G16" s="4">
+      <c r="F16" s="6">
         <v>0.31</v>
       </c>
-      <c r="H16" s="5">
+      <c r="G16" s="5">
         <v>25.898879749999999</v>
       </c>
-      <c r="I16" s="6">
+      <c r="H16" s="7">
         <v>473.50364624039224</v>
       </c>
-      <c r="J16" s="5">
+      <c r="I16" s="5">
         <v>715.65899999999999</v>
       </c>
-      <c r="K16" s="8">
+      <c r="J16" s="3">
         <v>47.573999999999998</v>
       </c>
-      <c r="L16" s="5">
+      <c r="K16" s="5">
         <v>12.79122222</v>
       </c>
-      <c r="M16" s="4">
+      <c r="L16" s="6">
         <v>7.88</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>2008</v>
       </c>
-      <c r="C17" s="2">
-        <v>66594.100999999995</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="C17" s="6">
         <v>811.03</v>
       </c>
-      <c r="E17" s="4">
+      <c r="D17" s="6">
         <v>32.06</v>
       </c>
-      <c r="F17" s="4">
+      <c r="E17" s="6">
         <v>0.42220000000000002</v>
       </c>
-      <c r="G17" s="4">
+      <c r="F17" s="6">
         <v>2.63</v>
       </c>
-      <c r="H17" s="5">
+      <c r="G17" s="5">
         <v>24.665748480000001</v>
       </c>
-      <c r="I17" s="6">
+      <c r="H17" s="7">
         <v>442.56096786732576</v>
       </c>
-      <c r="J17" s="5">
+      <c r="I17" s="5">
         <v>687.42499999999995</v>
       </c>
-      <c r="K17" s="8">
+      <c r="J17" s="3">
         <v>49.463000000000001</v>
       </c>
-      <c r="L17" s="5">
+      <c r="K17" s="5">
         <v>12.523968460000001</v>
       </c>
-      <c r="M17" s="4">
+      <c r="L17" s="6">
         <v>7.508</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I19" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analizy jednowymiarowe dla x1
</commit_message>
<xml_diff>
--- a/dane/Dane2.xlsx
+++ b/dane/Dane2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ja\Documents\GitHub\Ekonometria_projekt\dane\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\Ekonometria_projekt\dane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E379BA4-C1B6-4113-9A4F-0939FE9AB824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9081555F-7BF4-4014-BFE5-9296FC1CCBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1587B9EB-72E7-4C7E-BA4A-0E63A8296CF7}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1587B9EB-72E7-4C7E-BA4A-0E63A8296CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +108,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,10 +149,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -160,9 +168,12 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny 2" xfId="1" xr:uid="{AA3AB088-C57C-4061-AD90-EB762B6171C8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -178,9 +189,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office 2013–2022">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,7 +229,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office 2013–2022">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -324,7 +335,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office 2013–2022">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,7 +477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -474,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAF2763-4591-4F83-ACF8-5B34C9DC1611}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,6 +503,7 @@
     <col min="10" max="10" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.44140625" customWidth="1"/>
     <col min="12" max="13" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1102,7 +1114,7 @@
         <v>7.88</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1140,8 +1152,18 @@
         <v>7.508</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="X23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>